<commit_message>
Adding epsilon experiment for game with limited actions
</commit_message>
<xml_diff>
--- a/NormalResultsFindEpsilon(10kGames).xlsx
+++ b/NormalResultsFindEpsilon(10kGames).xlsx
@@ -2510,11 +2510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="217911680"/>
-        <c:axId val="217913600"/>
+        <c:axId val="78239616"/>
+        <c:axId val="78516224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="217911680"/>
+        <c:axId val="78239616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2544,12 +2544,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217913600"/>
+        <c:crossAx val="78516224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="217913600"/>
+        <c:axId val="78516224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="217911680"/>
+        <c:crossAx val="78239616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3284,11 +3284,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="168747776"/>
-        <c:axId val="166075392"/>
+        <c:axId val="78550912"/>
+        <c:axId val="78553088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="168747776"/>
+        <c:axId val="78550912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3318,13 +3318,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166075392"/>
+        <c:crossAx val="78553088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166075392"/>
+        <c:axId val="78553088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3354,7 +3354,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168747776"/>
+        <c:crossAx val="78550912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3725,9 +3725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -5490,7 +5488,7 @@
         <v>1257</v>
       </c>
       <c r="E98">
-        <f t="shared" ref="E98:E129" si="3">B98/SUM(B98:D98)</f>
+        <f t="shared" ref="E98:E100" si="3">B98/SUM(B98:D98)</f>
         <v>0.43930000000000002</v>
       </c>
     </row>

</xml_diff>